<commit_message>
count good nodes in binary tree
</commit_message>
<xml_diff>
--- a/Logics.xlsx
+++ b/Logics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit.raj\Desktop\SDE\DSA-github\leetcode_dsa-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B307D292-705D-4E9F-ADEE-D75178F99EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4576ED1F-C10D-4E42-9BB9-0D5105EDD17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1416" yWindow="936" windowWidth="21624" windowHeight="11304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="144">
   <si>
     <t>LOGIC</t>
   </si>
@@ -514,6 +514,18 @@
   </si>
   <si>
     <t>same logic as BFS traversal, jjust include at last in for loop as if(i == (size - 1)) { result.add(temp.val) ;} , because we have to add the value of last node present in the queue which will comes under our right view.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/construct-quad-tree/</t>
+  </si>
+  <si>
+    <t>create a helper method build for calling it recursively whenever some cell value doesn’t match. Take first cell value as reference and compare it inside for -for loop with other call vales, if at any point it doesn’t match break both loops with setting any flag like isSame=false. if isSame then return a noew node(fristVal==1, true). Else create four subgrids as topLeft, topRight,bottomLeft,bottomRight with new size =size/2 and passing the differennt values for row and col for each quadrant. At last return a new Node(true,false,tL,tR,bL,bR).</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/count-good-nodes-in-binary-tree/</t>
+  </si>
+  <si>
+    <t>Use DFS Preorder for traversal , keep track of max value after recursively call to process each node, and in a node is good Node if goodNode = node.val &gt;= maxVal?1:0.</t>
   </si>
 </sst>
 </file>
@@ -854,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O70"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="138" workbookViewId="0">
-      <selection activeCell="I70" sqref="I70"/>
+      <selection activeCell="I72" sqref="I72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1637,6 +1649,28 @@
       </c>
       <c r="I70" t="s">
         <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G71" t="s">
+        <v>4</v>
+      </c>
+      <c r="I71" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G72" t="s">
+        <v>4</v>
+      </c>
+      <c r="I72" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1691,6 +1725,8 @@
     <hyperlink ref="A68" r:id="rId48" xr:uid="{8AFF741F-6844-4DC1-877F-A827C07D6E01}"/>
     <hyperlink ref="A69" r:id="rId49" xr:uid="{E601C366-FE78-47A3-BF43-CDFB88B22095}"/>
     <hyperlink ref="A70" r:id="rId50" xr:uid="{28CEE045-F46F-408A-B6CB-9EC5D52A7A5C}"/>
+    <hyperlink ref="A71" r:id="rId51" xr:uid="{272B7ACC-9976-4AC5-8B77-C4E9CDF1E4E4}"/>
+    <hyperlink ref="A72" r:id="rId52" xr:uid="{2E7F7279-B158-4EE5-899E-93EB6239D89C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
kth smallest node in binary tree
</commit_message>
<xml_diff>
--- a/Logics.xlsx
+++ b/Logics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit.raj\Desktop\SDE\DSA-github\leetcode_dsa-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B3B50D-350E-4B83-815E-21EB360EEEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85868E9-F123-4D33-A6C2-1BEA39A31A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1416" yWindow="936" windowWidth="21624" windowHeight="11304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="148">
   <si>
     <t>LOGIC</t>
   </si>
@@ -532,6 +532,12 @@
   </si>
   <si>
     <t>use Long.MIN_VALUE and Long.MAX_VALUE to validate that every node value should come in this range, progressively the min =-infinity and max=node.val for left tree dfs and min=node.val ,max= + infinity for right dfs recursion. Make sure to return the result combinely for both left and right subtree recursion.I fwe observe in range updation , the left node value should always be less than the node.val and it may be anything which will lie in range of -inifinity to node.val, and vice-versa for right side child.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/kth-smallest-element-in-a-bst/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use DFS INORDER traversal , maintaina global counter so that it cant be reset every time in recursive call of function, with a var result to assign the node val if(counter ==k). Make dfsInorder as void and simply call it in kthSmallest method , and return result in kthSmallest.  </t>
   </si>
 </sst>
 </file>
@@ -872,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:O74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="138" workbookViewId="0">
-      <selection activeCell="I73" sqref="I73"/>
+      <selection activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1688,6 +1694,17 @@
       </c>
       <c r="I73" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G74" t="s">
+        <v>4</v>
+      </c>
+      <c r="I74" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1745,6 +1762,7 @@
     <hyperlink ref="A71" r:id="rId51" xr:uid="{272B7ACC-9976-4AC5-8B77-C4E9CDF1E4E4}"/>
     <hyperlink ref="A72" r:id="rId52" xr:uid="{2E7F7279-B158-4EE5-899E-93EB6239D89C}"/>
     <hyperlink ref="A73" r:id="rId53" xr:uid="{F518804A-3F12-4A18-83E4-78205DFD6391}"/>
+    <hyperlink ref="A74" r:id="rId54" xr:uid="{657559D3-11DB-4BE4-BA00-77F6780188EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
construct binary tree from preorder and inorder tree
</commit_message>
<xml_diff>
--- a/Logics.xlsx
+++ b/Logics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit.raj\Desktop\SDE\DSA-github\leetcode_dsa-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85868E9-F123-4D33-A6C2-1BEA39A31A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6878402-784B-4FBE-B18D-811194894918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="150">
   <si>
     <t>LOGIC</t>
   </si>
@@ -538,6 +538,12 @@
   </si>
   <si>
     <t xml:space="preserve">Use DFS INORDER traversal , maintaina global counter so that it cant be reset every time in recursive call of function, with a var result to assign the node val if(counter ==k). Make dfsInorder as void and simply call it in kthSmallest method , and return result in kthSmallest.  </t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/construct-binary-tree-from-preorder-and-inorder-traversal/</t>
+  </si>
+  <si>
+    <t>Traverse Preorder array and take its each element because it follows root-left-right, then find the index of each element in inorder (use map for storing the key as element and value=index for inorder array). After finding index split the inorder array recursively in left and right subtree, as root.left = build(pre,si,rootIndex-1), root.right=(pre,rootIndex+1,ei). At last return the rootNode.</t>
   </si>
 </sst>
 </file>
@@ -878,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O74"/>
+  <dimension ref="A1:O75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="138" workbookViewId="0">
-      <selection activeCell="I74" sqref="I74"/>
+      <selection activeCell="M64" sqref="M64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1705,6 +1711,17 @@
       </c>
       <c r="I74" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G75" t="s">
+        <v>4</v>
+      </c>
+      <c r="I75" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1763,6 +1780,7 @@
     <hyperlink ref="A72" r:id="rId52" xr:uid="{2E7F7279-B158-4EE5-899E-93EB6239D89C}"/>
     <hyperlink ref="A73" r:id="rId53" xr:uid="{F518804A-3F12-4A18-83E4-78205DFD6391}"/>
     <hyperlink ref="A74" r:id="rId54" xr:uid="{657559D3-11DB-4BE4-BA00-77F6780188EB}"/>
+    <hyperlink ref="A75" r:id="rId55" xr:uid="{7B8CDA49-0F1C-4B4D-A2E2-A1AD2028395E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
initial commmit for delete leaves with given node
</commit_message>
<xml_diff>
--- a/Logics.xlsx
+++ b/Logics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit.raj\Desktop\SDE\DSA-github\leetcode_dsa-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A093D9E-914A-4EBC-A17C-A5DB7D6546DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736DE100-3D6D-4449-B431-F2E9F2DD23E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="153">
   <si>
     <t>LOGIC</t>
   </si>
@@ -550,6 +550,9 @@
   </si>
   <si>
     <t>Use modified DFS approach, we can only rob the node in two ways, either from root, root.left.left, root.left.right and root, root.right.right, root.right.left. Basicallly use pair approach [withRoot,withoutRoot], in which the withRoot=root.val+leftPair[1]+rightPair[1], withoutRoot= max(leftPair[0],leftPair[1])+max(rightPair[0],rightPair[1]). At last return the max of pair using max(pair[0],pair[1]).</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/delete-leaves-with-a-given-value/</t>
   </si>
 </sst>
 </file>
@@ -890,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O76"/>
+  <dimension ref="A1:O77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="138" workbookViewId="0">
-      <selection activeCell="I76" sqref="I76"/>
+      <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1739,6 +1742,14 @@
       </c>
       <c r="I76" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G77" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1799,6 +1810,7 @@
     <hyperlink ref="A74" r:id="rId54" xr:uid="{657559D3-11DB-4BE4-BA00-77F6780188EB}"/>
     <hyperlink ref="A75" r:id="rId55" xr:uid="{7B8CDA49-0F1C-4B4D-A2E2-A1AD2028395E}"/>
     <hyperlink ref="A76" r:id="rId56" xr:uid="{5232C98D-B5FC-41AC-9721-C3ACDD2C931E}"/>
+    <hyperlink ref="A77" r:id="rId57" xr:uid="{AEEBD9EE-05FF-467C-9357-F612421405CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
delete leaf nodes with given target
</commit_message>
<xml_diff>
--- a/Logics.xlsx
+++ b/Logics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit.raj\Desktop\SDE\DSA-github\leetcode_dsa-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736DE100-3D6D-4449-B431-F2E9F2DD23E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909E6AC5-C5F7-4B97-BD33-A2B54B08FABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="154">
   <si>
     <t>LOGIC</t>
   </si>
@@ -553,6 +553,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/delete-leaves-with-a-given-value/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use DFS(PostOrder) because we need to check the node before processing , because we will not going to know whether this node has to be removed or not if we will use preorder or inorder. With if(root.left==null &amp;&amp; root.right==null &amp;&amp; root.val==val) then return null for the current node to simply delete or remove it. Else at last return that node means we have to keep the current node because its not the leaf with matching the target. </t>
   </si>
 </sst>
 </file>
@@ -896,7 +899,7 @@
   <dimension ref="A1:O77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="138" workbookViewId="0">
-      <selection activeCell="G77" sqref="G77"/>
+      <selection activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1750,6 +1753,9 @@
       </c>
       <c r="G77" t="s">
         <v>4</v>
+      </c>
+      <c r="I77" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kth largest element using heap
</commit_message>
<xml_diff>
--- a/Logics.xlsx
+++ b/Logics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit.raj\Desktop\SDE\DSA-github\leetcode_dsa-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909E6AC5-C5F7-4B97-BD33-A2B54B08FABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD0C48A-8F48-4BEC-9292-4002B0DB2CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="156">
   <si>
     <t>LOGIC</t>
   </si>
@@ -556,6 +556,12 @@
   </si>
   <si>
     <t xml:space="preserve">Use DFS(PostOrder) because we need to check the node before processing , because we will not going to know whether this node has to be removed or not if we will use preorder or inorder. With if(root.left==null &amp;&amp; root.right==null &amp;&amp; root.val==val) then return null for the current node to simply delete or remove it. Else at last return that node means we have to keep the current node because its not the leaf with matching the target. </t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/kth-largest-element-in-a-stream/</t>
+  </si>
+  <si>
+    <t>Use minHeap priorityQueue, so here we will maintain the the heap size as k and polling the element if(heap.size()&gt;k) at any instNt. So by doing this, the kth largest element will always be the root or say on the top which will be peeked() to return the result.</t>
   </si>
 </sst>
 </file>
@@ -896,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O77"/>
+  <dimension ref="A1:O78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="138" workbookViewId="0">
-      <selection activeCell="I77" sqref="I77"/>
+      <selection activeCell="I78" sqref="I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1756,6 +1762,17 @@
       </c>
       <c r="I77" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G78" t="s">
+        <v>4</v>
+      </c>
+      <c r="I78" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1817,6 +1834,7 @@
     <hyperlink ref="A75" r:id="rId55" xr:uid="{7B8CDA49-0F1C-4B4D-A2E2-A1AD2028395E}"/>
     <hyperlink ref="A76" r:id="rId56" xr:uid="{5232C98D-B5FC-41AC-9721-C3ACDD2C931E}"/>
     <hyperlink ref="A77" r:id="rId57" xr:uid="{AEEBD9EE-05FF-467C-9357-F612421405CF}"/>
+    <hyperlink ref="A78" r:id="rId58" xr:uid="{5067DA5A-74E3-4E8B-8389-9AF891FE4F8E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
k closest points to origin
</commit_message>
<xml_diff>
--- a/Logics.xlsx
+++ b/Logics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit.raj\Desktop\SDE\DSA-github\leetcode_dsa-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181C86FA-0D88-41A2-99BF-44F1FD2CC5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEEDEB9-D233-412D-97D5-81F73CF960D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="159">
   <si>
     <t>LOGIC</t>
   </si>
@@ -568,6 +568,9 @@
   </si>
   <si>
     <t>Use maxHeap priorityQueue for solving ths problem, first add all elements to pq then run while loop until pq.size()&gt;1 because we have smash the stones until 0 or 1 stone remains.In while , add the diff to pq only when its &gt; 0 because in case of 0 the stone has been smashed .Return the peeked element if pq.size()&gt;0 else 0 means all stones smashed.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/k-closest-points-to-origin/</t>
   </si>
 </sst>
 </file>
@@ -908,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O79"/>
+  <dimension ref="A1:O80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="138" workbookViewId="0">
-      <selection activeCell="I79" sqref="I79"/>
+      <selection activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1790,6 +1793,11 @@
       </c>
       <c r="I79" t="s">
         <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" s="2" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1853,6 +1861,7 @@
     <hyperlink ref="A77" r:id="rId57" xr:uid="{AEEBD9EE-05FF-467C-9357-F612421405CF}"/>
     <hyperlink ref="A78" r:id="rId58" xr:uid="{5067DA5A-74E3-4E8B-8389-9AF891FE4F8E}"/>
     <hyperlink ref="A79" r:id="rId59" xr:uid="{83A5A060-EFB2-4D85-B182-84E335410FFA}"/>
+    <hyperlink ref="A80" r:id="rId60" xr:uid="{48EF1115-DF39-4B1C-88FB-BD3842A18151}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
logic updation for k closest points to origin
</commit_message>
<xml_diff>
--- a/Logics.xlsx
+++ b/Logics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit.raj\Desktop\SDE\DSA-github\leetcode_dsa-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEEDEB9-D233-412D-97D5-81F73CF960D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78452F38-377F-49CB-803C-5CDF5C1B265E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="160">
   <si>
     <t>LOGIC</t>
   </si>
@@ -571,6 +571,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/k-closest-points-to-origin/</t>
+  </si>
+  <si>
+    <t>we will sort the heap or PQ in descending order to maintain the k closest points to the origin. Loop the points array , take current and find the dist between the points, then offer it to pq with the index of the current array in points 2d arrray, so that we can access the inner array to store it in result. After offering, if pq.size()&gt; k then poll it. So we are sorting the pq in descending order it means the farthest point form the origin will always be on top and will be remoed continously whenever a closest points to the origin will be added to PQ.</t>
   </si>
 </sst>
 </file>
@@ -914,7 +917,7 @@
   <dimension ref="A1:O80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="138" workbookViewId="0">
-      <selection activeCell="I71" sqref="I71"/>
+      <selection activeCell="I80" sqref="I80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1798,6 +1801,12 @@
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>158</v>
+      </c>
+      <c r="G80" t="s">
+        <v>4</v>
+      </c>
+      <c r="I80" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kth largest element in an array
</commit_message>
<xml_diff>
--- a/Logics.xlsx
+++ b/Logics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit.raj\Desktop\SDE\DSA-github\leetcode_dsa-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78452F38-377F-49CB-803C-5CDF5C1B265E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A01D9C-25B1-4CF2-916A-0E87575A070F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="162">
   <si>
     <t>LOGIC</t>
   </si>
@@ -574,6 +574,12 @@
   </si>
   <si>
     <t>we will sort the heap or PQ in descending order to maintain the k closest points to the origin. Loop the points array , take current and find the dist between the points, then offer it to pq with the index of the current array in points 2d arrray, so that we can access the inner array to store it in result. After offering, if pq.size()&gt; k then poll it. So we are sorting the pq in descending order it means the farthest point form the origin will always be on top and will be remoed continously whenever a closest points to the origin will be added to PQ.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/kth-largest-element-in-an-array/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use minHeap so that the minimum element will be at top and get removed whenever a new element will be added to maintain the heap size of k largest elements with this we will get the kth largest element at top after traversing all the elements in the array with maintaining the size of pq of k. </t>
   </si>
 </sst>
 </file>
@@ -914,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O80"/>
+  <dimension ref="A1:O81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="138" workbookViewId="0">
-      <selection activeCell="I80" sqref="I80"/>
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1807,6 +1813,17 @@
       </c>
       <c r="I80" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G81" t="s">
+        <v>4</v>
+      </c>
+      <c r="I81" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1871,6 +1888,7 @@
     <hyperlink ref="A78" r:id="rId58" xr:uid="{5067DA5A-74E3-4E8B-8389-9AF891FE4F8E}"/>
     <hyperlink ref="A79" r:id="rId59" xr:uid="{83A5A060-EFB2-4D85-B182-84E335410FFA}"/>
     <hyperlink ref="A80" r:id="rId60" xr:uid="{48EF1115-DF39-4B1C-88FB-BD3842A18151}"/>
+    <hyperlink ref="A81" r:id="rId61" xr:uid="{C2414E4E-43A9-4C6D-B40C-7ACB14F51A12}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
task scheduler using maxHeap
</commit_message>
<xml_diff>
--- a/Logics.xlsx
+++ b/Logics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit.raj\Desktop\SDE\DSA-github\leetcode_dsa-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A01D9C-25B1-4CF2-916A-0E87575A070F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190A2ADB-C82A-4747-9D08-F074C4C7B5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="164">
   <si>
     <t>LOGIC</t>
   </si>
@@ -580,6 +580,12 @@
   </si>
   <si>
     <t xml:space="preserve">Use minHeap so that the minimum element will be at top and get removed whenever a new element will be added to maintain the heap size of k largest elements with this we will get the kth largest element at top after traversing all the elements in the array with maintaining the size of pq of k. </t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/task-scheduler/</t>
+  </si>
+  <si>
+    <t>First use hashmap to store the frequency of each character, then use maxHeap for storing the frequencies by getting from map.values() in decreasing order. Track of interval and increment it in looping till while(!pq.isEmpty() || queue.isEMpty(). Use a queue for cooldown period for storing the freq with the ready time for it. After processing each task from heap , then check in cooldown period queue and add the freq which have readyTIme == currentTIme , back to heap for processing again. Make sure while adding to coolDown period that remFreq should be greater than 1 otherwise its of no use to put in cooldown period.</t>
   </si>
 </sst>
 </file>
@@ -920,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O81"/>
+  <dimension ref="A1:O82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="138" workbookViewId="0">
-      <selection activeCell="I81" sqref="I81"/>
+      <selection activeCell="I82" sqref="I82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1824,6 +1830,17 @@
       </c>
       <c r="I81" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G82" t="s">
+        <v>4</v>
+      </c>
+      <c r="I82" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1889,6 +1906,7 @@
     <hyperlink ref="A79" r:id="rId59" xr:uid="{83A5A060-EFB2-4D85-B182-84E335410FFA}"/>
     <hyperlink ref="A80" r:id="rId60" xr:uid="{48EF1115-DF39-4B1C-88FB-BD3842A18151}"/>
     <hyperlink ref="A81" r:id="rId61" xr:uid="{C2414E4E-43A9-4C6D-B40C-7ACB14F51A12}"/>
+    <hyperlink ref="A82" r:id="rId62" xr:uid="{E2BDA73C-C558-45BC-BF45-F17949C4200B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
all combination from the range
</commit_message>
<xml_diff>
--- a/Logics.xlsx
+++ b/Logics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit.raj\Desktop\SDE\DSA-github\leetcode_dsa-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A590D1BC-AF55-4495-916A-39A6D2436BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C52C2E-D82D-49B4-BF5F-15D3EC30C5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="184">
   <si>
     <t>LOGIC</t>
   </si>
@@ -640,6 +640,12 @@
   </si>
   <si>
     <t>same as combinations sum, but make sure of these points. Sort the candidate array first, inside backtrack run a for loop and inside it check for duplicates, if found then continue also if target &gt; cand[i] then break because then combinations are not possible. Call backtrack once only after including the cand[i] with index as i + 1, because now we have to check for another element to create the combination.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/combinations/</t>
+  </si>
+  <si>
+    <t>Same logics of include backtrack and exclude, Base case will be if current.size() == k then include it to result and return. Later run a for loop from start to end, inside the loop , first include the element to current then backtrack with i+1 as we have to build combination of i and all other elements present in the range, at last exclude the last added element or simpky undo the last step.</t>
   </si>
 </sst>
 </file>
@@ -980,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O91"/>
+  <dimension ref="A1:O92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B78" zoomScale="138" workbookViewId="0">
-      <selection activeCell="I91" sqref="I91"/>
+      <selection activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1994,6 +2000,17 @@
       </c>
       <c r="I91" t="s">
         <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
+        <v>182</v>
+      </c>
+      <c r="G92" t="s">
+        <v>4</v>
+      </c>
+      <c r="I92" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generate parenthesis detailed logic
</commit_message>
<xml_diff>
--- a/Logics.xlsx
+++ b/Logics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit.raj\Desktop\SDE\DSA-github\leetcode_dsa-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5832704-8FB3-4D7A-A671-1908F7A9E5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD54350D-3254-43AD-BF92-9825029D63A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -669,7 +669,7 @@
     <t>https://leetcode.com/problems/word-search/</t>
   </si>
   <si>
-    <t>This solution uses backtracking to generate all valid combinations of parentheses. It keeps track of how many opening and closing brackets have been used so far. At each step, it adds an opening bracket if it’s still allowed, or a closing bracket if it keeps the string valid. When the current string reaches twice the length of n, it’s added to the final list as a valid combination.</t>
+    <t>This solution uses backtracking to generate all valid combinations of parentheses. It keeps track of how many opening and closing brackets have been used so far. At each step, it adds an opening bracket if it’s still allowed, or a closing bracket if it keeps the string valid. When the current string reaches twice the length of n, it’s added to the final list as a valid combination. so mostly take care of two conditions while adding the open braces (open&lt;=max) and close braces (close&lt;=open), while calling the recursion for both separately, because for addition of both we have separate conditions and requirements.</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
letter combinations of a phone number
</commit_message>
<xml_diff>
--- a/Logics.xlsx
+++ b/Logics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit.raj\Desktop\SDE\DSA-github\leetcode_dsa-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E13E92-CEE8-4ABC-9DA3-1FB946951A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE9C935-0C2F-4258-9D56-D89A5FB873B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="197">
   <si>
     <t>LOGIC</t>
   </si>
@@ -676,6 +676,15 @@
   </si>
   <si>
     <t>This solution uses DFS with backtracking to check if a given word can be formed by sequentially adjacent letters in the grid.It starts a recursive search from every cell matching the word’s first letter, exploring in all four directions (up, down, left, right).Each visited cell is temporarily marked to prevent reuse within the same path, then unmarked (backtracked) after exploration.The recursion succeeds if all characters in the word are found consecutively and returns true once a full match is formed.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/letter-combinations-of-a-phone-number/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a boolean 2*2 matrix to keep track of whether the range start..end is palindrome or not. Base case will be ,if start reaches at last means at the string length()-1 then return. In recursion we run loop to expand the substring from the current start , inside the loop we check for the condition as (s.charAt(start) == s.charAt(end) &amp;&amp; (end - start &lt;= 2 || dp[start + 1][end - 1])), means if start and end char matches then either it should be of lenght less than or equal to 2 or it is marked as palindrome in the boolean matrix., then similar steps as, marked the current substring as palindrom in matrix, add that to current path, call recursion with end+1 ast start for next stackframe, then undo the last step on rturning. </t>
+  </si>
+  <si>
+    <t>Create a map to store the character as key with their correspoinding values, base case will be if the index (using to iterate or keep track of each character in given digits) ==digits.length() means we are at last char of digits. Then fetch the current char using index, then fetch its corresponding value, then run a for loop for each char present in that digit value to make all the possible combination, inside loop just call the recursive method with incrementing the index as we have explore other options with the current char, and with concatening the current char (c) with the current path.</t>
   </si>
 </sst>
 </file>
@@ -1016,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O98"/>
+  <dimension ref="A1:O99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="138" workbookViewId="0">
-      <selection activeCell="I96" sqref="I96"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="138" workbookViewId="0">
+      <selection activeCell="I99" sqref="I99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2104,6 +2113,20 @@
       </c>
       <c r="G98" t="s">
         <v>4</v>
+      </c>
+      <c r="I98" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G99" t="s">
+        <v>4</v>
+      </c>
+      <c r="I99" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -2184,6 +2207,7 @@
     <hyperlink ref="B95" r:id="rId74" xr:uid="{CF7A17BF-E8F3-4C8B-9A65-A768BC783EF9}"/>
     <hyperlink ref="B96" r:id="rId75" xr:uid="{3C985415-142A-4BEC-B75D-EB7C7CC768E8}"/>
     <hyperlink ref="A97" r:id="rId76" xr:uid="{73E01CDD-735E-4623-A26B-9B0924A37B06}"/>
+    <hyperlink ref="A99" r:id="rId77" xr:uid="{EFEF0D6A-A2F3-456C-A490-89AF4FAA8F5F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
partition to equal k sum logix changes
</commit_message>
<xml_diff>
--- a/Logics.xlsx
+++ b/Logics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit.raj\Desktop\SDE\DSA-github\leetcode_dsa-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A73E5F8-7BA6-4589-AFF8-BD75843A8537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6BCAC4-5994-4C89-AE8E-7EB6C87F3411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1416" yWindow="936" windowWidth="21624" windowHeight="11304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="200">
   <si>
     <t>LOGIC</t>
   </si>
@@ -691,6 +691,9 @@
   </si>
   <si>
     <t>1.First, compute the total sum of all matchsticks — if it’s not divisible by 4, return false.2.Each side of the square must have a length of sum / 4. 3️.Sort the sticks in descending order to try longer ones first (helps prune impossible paths).4️.Use backtracking to assign each stick to one of 4 sides, ensuring no side exceeds the target length.5️.If all sticks are used and all sides equal the target, return true; otherwise, backtrack and try again.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/partition-to-k-equal-sum-subsets/</t>
   </si>
 </sst>
 </file>
@@ -1031,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O100"/>
+  <dimension ref="A1:O101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A92" zoomScale="138" workbookViewId="0">
-      <selection activeCell="I100" sqref="I100"/>
+      <selection activeCell="H101" sqref="H101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2144,6 +2147,14 @@
       </c>
       <c r="I100" t="s">
         <v>198</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G101" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2226,6 +2237,7 @@
     <hyperlink ref="A97" r:id="rId76" xr:uid="{73E01CDD-735E-4623-A26B-9B0924A37B06}"/>
     <hyperlink ref="A99" r:id="rId77" xr:uid="{EFEF0D6A-A2F3-456C-A490-89AF4FAA8F5F}"/>
     <hyperlink ref="A100" r:id="rId78" xr:uid="{27B6E1F3-5A51-4799-A52D-0E00ECF9057E}"/>
+    <hyperlink ref="A101" r:id="rId79" xr:uid="{BBCECA0C-7F19-47DD-ACD3-DF51E2D86AF5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
partitioning to k equal sums
</commit_message>
<xml_diff>
--- a/Logics.xlsx
+++ b/Logics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit.raj\Desktop\SDE\DSA-github\leetcode_dsa-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6BCAC4-5994-4C89-AE8E-7EB6C87F3411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD65DA1B-0B81-4D73-8451-4E15C46609C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1416" yWindow="936" windowWidth="21624" windowHeight="11304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="201">
   <si>
     <t>LOGIC</t>
   </si>
@@ -694,6 +694,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/partition-to-k-equal-sum-subsets/</t>
+  </si>
+  <si>
+    <t>1.Calculate the total sum — if not divisible by k, return false.2️.Target per subset = total / k.3️.Use boolean[] used to track which elements are already in subsets.4️.Backtrack to fill subsets until each equals the target, then move to the next subset.5️.When k == 1, return true (remaining numbers form the last valid subset).</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1040,7 @@
   <dimension ref="A1:O101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A92" zoomScale="138" workbookViewId="0">
-      <selection activeCell="H101" sqref="H101"/>
+      <selection activeCell="I101" sqref="I101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2155,6 +2158,9 @@
       </c>
       <c r="G101" t="s">
         <v>4</v>
+      </c>
+      <c r="I101" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trie Implementation with logic
</commit_message>
<xml_diff>
--- a/Logics.xlsx
+++ b/Logics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit.raj\Desktop\SDE\DSA-github\leetcode_dsa-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3550B39F-FC90-4D4B-90EC-54CB6BEC1BD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431B058D-F4DC-47BB-8066-86644227A6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1416" yWindow="936" windowWidth="21624" windowHeight="11304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="203">
   <si>
     <t>LOGIC</t>
   </si>
@@ -700,6 +700,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/implement-trie-prefix-tree/</t>
+  </si>
+  <si>
+    <t>Each character of a word is stored as a path in a tree where every node has 26 possible children (a–z).insert() builds this path by creating missing nodes and marking the last node as an end-of-word.search() follows the same path and returns true only if the entire path exists and the final node is marked as an end-of-word.startsWith() checks only whether the prefix path exists, without needing the end-of-word flag.</t>
   </si>
 </sst>
 </file>
@@ -1042,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="138" workbookViewId="0">
-      <selection activeCell="I102" sqref="I102"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="138" workbookViewId="0">
+      <selection activeCell="J102" sqref="J102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2111,7 +2114,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>40</v>
       </c>
@@ -2122,7 +2125,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>192</v>
       </c>
@@ -2133,7 +2136,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>194</v>
       </c>
@@ -2144,7 +2147,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>197</v>
       </c>
@@ -2155,7 +2158,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>199</v>
       </c>
@@ -2166,15 +2169,15 @@
         <v>200</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>201</v>
       </c>
       <c r="G102" t="s">
         <v>4</v>
       </c>
-      <c r="I102">
-        <v>1</v>
+      <c r="J102" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>